<commit_message>
continued working on series code
</commit_message>
<xml_diff>
--- a/SDG-Matrix/Output/series_catalog.xlsx
+++ b/SDG-Matrix/Output/series_catalog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3983" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4019" uniqueCount="807">
   <si>
     <t>GOAL</t>
   </si>
@@ -2463,6 +2463,72 @@
   </si>
   <si>
     <t>DC_TOF_TRDDBML</t>
+  </si>
+  <si>
+    <t>NV_IND_MANF</t>
+  </si>
+  <si>
+    <t>NV_IND_MANFPC</t>
+  </si>
+  <si>
+    <t>SL_TLF_MANF</t>
+  </si>
+  <si>
+    <t>NV_IND_SSIS</t>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color rgb="FF777777"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GB_POP_SCIERD</t>
+    </r>
+  </si>
+  <si>
+    <t>EN_ATM_CO2</t>
+  </si>
+  <si>
+    <t>NV_IND_TECH</t>
+  </si>
+  <si>
+    <t>IT_MOB_NTWK</t>
+  </si>
+  <si>
+    <t>SI_HEI_TOTL</t>
+  </si>
+  <si>
+    <t>SI_RMT_COST</t>
+  </si>
+  <si>
+    <t>SG_SCP_CNTRY</t>
+  </si>
+  <si>
+    <t>AG_LND_FRST</t>
+  </si>
+  <si>
+    <t>ER_PTD_TERRS</t>
+  </si>
+  <si>
+    <t>ER_PTD_MOTN</t>
+  </si>
+  <si>
+    <t>ER_MTN_GRNCVI</t>
+  </si>
+  <si>
+    <t>ER_RSK_LSTI</t>
+  </si>
+  <si>
+    <t>DC_ODA_BDVDL</t>
+  </si>
+  <si>
+    <t>VC_IHR_PSRCN</t>
   </si>
 </sst>
 </file>
@@ -2552,7 +2618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2566,6 +2632,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2907,9 +2974,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AJ296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="11" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A193" sqref="A193:XFD195"/>
+      <selection pane="topRight" activeCell="J234" sqref="J234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8966,7 +9033,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="140" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:36" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>42</v>
       </c>
@@ -9010,7 +9077,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="141" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:36" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>42</v>
       </c>
@@ -9057,7 +9124,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="142" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:36" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>42</v>
       </c>
@@ -9104,7 +9171,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="143" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:36" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>42</v>
       </c>
@@ -9148,7 +9215,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="144" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:36" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>42</v>
       </c>
@@ -9192,7 +9259,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="145" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>42</v>
       </c>
@@ -9236,7 +9303,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="146" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>42</v>
       </c>
@@ -9280,7 +9347,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="147" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>42</v>
       </c>
@@ -9327,7 +9394,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="148" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>42</v>
       </c>
@@ -9371,7 +9438,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="149" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>42</v>
       </c>
@@ -9415,7 +9482,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="150" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>42</v>
       </c>
@@ -9459,7 +9526,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="151" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>42</v>
       </c>
@@ -9506,7 +9573,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="152" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>42</v>
       </c>
@@ -9553,7 +9620,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="153" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>42</v>
       </c>
@@ -9600,7 +9667,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="154" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>42</v>
       </c>
@@ -9647,7 +9714,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="155" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>42</v>
       </c>
@@ -9694,7 +9761,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="156" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>42</v>
       </c>
@@ -9741,7 +9808,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="157" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>42</v>
       </c>
@@ -9788,7 +9855,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="158" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>42</v>
       </c>
@@ -9835,7 +9902,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="159" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>42</v>
       </c>
@@ -9882,7 +9949,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="160" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>42</v>
       </c>
@@ -9929,7 +9996,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="161" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>42</v>
       </c>
@@ -9976,7 +10043,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="162" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>42</v>
       </c>
@@ -10023,7 +10090,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="163" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>42</v>
       </c>
@@ -10070,7 +10137,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="164" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>42</v>
       </c>
@@ -10117,7 +10184,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="165" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>42</v>
       </c>
@@ -10161,7 +10228,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="166" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>42</v>
       </c>
@@ -10205,7 +10272,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="167" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>42</v>
       </c>
@@ -10249,7 +10316,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="168" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>42</v>
       </c>
@@ -10293,7 +10360,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="169" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>42</v>
       </c>
@@ -10337,7 +10404,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="170" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>42</v>
       </c>
@@ -10381,7 +10448,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="171" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>42</v>
       </c>
@@ -10425,7 +10492,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="172" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>42</v>
       </c>
@@ -10469,7 +10536,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="173" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>42</v>
       </c>
@@ -10513,7 +10580,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="174" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>42</v>
       </c>
@@ -10557,7 +10624,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="175" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>42</v>
       </c>
@@ -10601,7 +10668,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="176" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>42</v>
       </c>
@@ -10645,7 +10712,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="177" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>42</v>
       </c>
@@ -10689,7 +10756,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="178" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>42</v>
       </c>
@@ -10733,7 +10800,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="179" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>42</v>
       </c>
@@ -10777,7 +10844,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="180" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>42</v>
       </c>
@@ -10821,7 +10888,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="181" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>42</v>
       </c>
@@ -10865,7 +10932,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="182" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>42</v>
       </c>
@@ -10909,7 +10976,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="183" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>42</v>
       </c>
@@ -10953,7 +11020,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="184" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>42</v>
       </c>
@@ -10997,7 +11064,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="185" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>42</v>
       </c>
@@ -11041,7 +11108,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="186" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:34" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="5" t="s">
         <v>42</v>
       </c>
@@ -11084,7 +11151,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="187" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:34" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" s="5" t="s">
         <v>42</v>
       </c>
@@ -11130,7 +11197,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="188" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:34" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" s="5" t="s">
         <v>42</v>
       </c>
@@ -11176,7 +11243,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="189" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:34" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" s="5" t="s">
         <v>42</v>
       </c>
@@ -11222,7 +11289,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="190" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:34" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" s="5" t="s">
         <v>42</v>
       </c>
@@ -11265,7 +11332,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="191" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:34" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" s="5" t="s">
         <v>42</v>
       </c>
@@ -11308,7 +11375,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="192" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:34" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" s="8" t="s">
         <v>42</v>
       </c>
@@ -11351,7 +11418,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="193" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:36" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" s="8" t="s">
         <v>42</v>
       </c>
@@ -11400,7 +11467,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="194" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:36" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" s="8" t="s">
         <v>42</v>
       </c>
@@ -11446,7 +11513,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="195" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:36" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" s="8" t="s">
         <v>42</v>
       </c>
@@ -11520,6 +11587,9 @@
       <c r="J196" t="s">
         <v>417</v>
       </c>
+      <c r="K196" s="4" t="s">
+        <v>789</v>
+      </c>
       <c r="L196" t="s">
         <v>511</v>
       </c>
@@ -11564,6 +11634,9 @@
       <c r="J197" t="s">
         <v>417</v>
       </c>
+      <c r="K197" s="4" t="s">
+        <v>790</v>
+      </c>
       <c r="L197" t="s">
         <v>512</v>
       </c>
@@ -11608,6 +11681,9 @@
       <c r="J198" t="s">
         <v>417</v>
       </c>
+      <c r="K198" s="4" t="s">
+        <v>789</v>
+      </c>
       <c r="L198" t="s">
         <v>511</v>
       </c>
@@ -11652,6 +11728,9 @@
       <c r="J199" t="s">
         <v>418</v>
       </c>
+      <c r="K199" s="4" t="s">
+        <v>791</v>
+      </c>
       <c r="L199" t="s">
         <v>513</v>
       </c>
@@ -11693,6 +11772,9 @@
       <c r="J200" t="s">
         <v>418</v>
       </c>
+      <c r="K200" s="4" t="s">
+        <v>791</v>
+      </c>
       <c r="L200" t="s">
         <v>513</v>
       </c>
@@ -11734,6 +11816,9 @@
       <c r="J201" t="s">
         <v>418</v>
       </c>
+      <c r="K201" s="4" t="s">
+        <v>791</v>
+      </c>
       <c r="L201" t="s">
         <v>513</v>
       </c>
@@ -11775,6 +11860,9 @@
       <c r="J202" t="s">
         <v>419</v>
       </c>
+      <c r="K202" s="4" t="s">
+        <v>792</v>
+      </c>
       <c r="L202" t="s">
         <v>514</v>
       </c>
@@ -11816,6 +11904,9 @@
       <c r="J203" t="s">
         <v>420</v>
       </c>
+      <c r="K203" s="4" t="s">
+        <v>794</v>
+      </c>
       <c r="L203" t="s">
         <v>515</v>
       </c>
@@ -11857,6 +11948,9 @@
       <c r="J204" t="s">
         <v>421</v>
       </c>
+      <c r="K204" s="7" t="s">
+        <v>793</v>
+      </c>
       <c r="L204" t="s">
         <v>516</v>
       </c>
@@ -11898,6 +11992,9 @@
       <c r="J205" t="s">
         <v>422</v>
       </c>
+      <c r="K205" s="4" t="s">
+        <v>795</v>
+      </c>
       <c r="L205" t="s">
         <v>517</v>
       </c>
@@ -11939,6 +12036,9 @@
       <c r="J206" t="s">
         <v>422</v>
       </c>
+      <c r="K206" s="4" t="s">
+        <v>795</v>
+      </c>
       <c r="L206" t="s">
         <v>517</v>
       </c>
@@ -11980,6 +12080,9 @@
       <c r="J207" t="s">
         <v>423</v>
       </c>
+      <c r="K207" s="4" t="s">
+        <v>796</v>
+      </c>
       <c r="L207" t="s">
         <v>518</v>
       </c>
@@ -11996,41 +12099,46 @@
         <v>714</v>
       </c>
     </row>
-    <row r="208" spans="1:36" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A208" t="s">
+    <row r="208" spans="1:36" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A208" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B208" t="s">
         <v>57</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C208" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="F208" t="s">
+      <c r="E208"/>
+      <c r="F208" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="G208" t="s">
+      <c r="G208" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="H208" t="s">
+      <c r="H208" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="J208" t="s">
+      <c r="I208"/>
+      <c r="J208" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="L208" t="s">
+      <c r="K208" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="L208" s="8" t="s">
         <v>519</v>
       </c>
-      <c r="AB208" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="AC208" t="s">
+      <c r="AB208" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="AC208" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="AH208" t="s">
+      <c r="AH208" s="8" t="s">
         <v>706</v>
       </c>
     </row>
@@ -12059,6 +12167,9 @@
       <c r="J209" t="s">
         <v>425</v>
       </c>
+      <c r="K209" s="4" t="s">
+        <v>798</v>
+      </c>
       <c r="L209" t="s">
         <v>520</v>
       </c>
@@ -12094,6 +12205,9 @@
       <c r="J210" t="s">
         <v>426</v>
       </c>
+      <c r="K210" s="4" t="s">
+        <v>738</v>
+      </c>
       <c r="L210" t="s">
         <v>521</v>
       </c>
@@ -12135,6 +12249,9 @@
       <c r="J211" t="s">
         <v>426</v>
       </c>
+      <c r="K211" s="4" t="s">
+        <v>736</v>
+      </c>
       <c r="L211" t="s">
         <v>522</v>
       </c>
@@ -12176,6 +12293,9 @@
       <c r="J212" t="s">
         <v>426</v>
       </c>
+      <c r="K212" s="4" t="s">
+        <v>737</v>
+      </c>
       <c r="L212" t="s">
         <v>523</v>
       </c>
@@ -12217,6 +12337,9 @@
       <c r="J213" t="s">
         <v>427</v>
       </c>
+      <c r="K213" s="4" t="s">
+        <v>740</v>
+      </c>
       <c r="L213" t="s">
         <v>524</v>
       </c>
@@ -12236,346 +12359,380 @@
         <v>714</v>
       </c>
     </row>
-    <row r="214" spans="1:36" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A214" t="s">
+    <row r="214" spans="1:36" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A214" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B214" t="s">
         <v>59</v>
       </c>
-      <c r="C214" t="s">
+      <c r="C214" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D214" t="s">
+      <c r="D214" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="F214" t="s">
+      <c r="E214"/>
+      <c r="F214" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="G214" t="s">
+      <c r="G214" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="H214" t="s">
+      <c r="H214" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="J214" t="s">
+      <c r="I214"/>
+      <c r="J214" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="L214" t="s">
+      <c r="K214" s="9" t="s">
+        <v>799</v>
+      </c>
+      <c r="L214" s="8" t="s">
         <v>525</v>
       </c>
-      <c r="AB214" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="AD214" t="s">
+      <c r="AB214" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="AD214" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="AH214" t="s">
+      <c r="AH214" s="8" t="s">
         <v>720</v>
       </c>
-      <c r="AJ214" t="s">
+      <c r="AJ214" s="8" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="215" spans="1:36" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A215" t="s">
+    <row r="215" spans="1:36" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A215" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B215" t="s">
         <v>59</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C215" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D215" t="s">
+      <c r="D215" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F215" t="s">
+      <c r="E215"/>
+      <c r="F215" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="G215" t="s">
+      <c r="G215" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="H215" t="s">
+      <c r="H215" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="J215" t="s">
+      <c r="I215"/>
+      <c r="J215" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="L215" t="s">
+      <c r="L215" s="5" t="s">
         <v>526</v>
       </c>
-      <c r="AB215" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="AD215" t="s">
+      <c r="AB215" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="AD215" s="5" t="s">
         <v>698</v>
       </c>
-      <c r="AH215" t="s">
+      <c r="AH215" s="5" t="s">
         <v>721</v>
       </c>
-      <c r="AJ215" t="s">
+      <c r="AJ215" s="5" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="216" spans="1:36" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A216" t="s">
+    <row r="216" spans="1:36" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A216" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B216" t="s">
         <v>59</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C216" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F216" t="s">
+      <c r="E216"/>
+      <c r="F216" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="G216" t="s">
+      <c r="G216" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="H216" t="s">
+      <c r="H216" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="J216" t="s">
+      <c r="I216"/>
+      <c r="J216" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="L216" t="s">
+      <c r="L216" s="5" t="s">
         <v>526</v>
       </c>
-      <c r="AB216" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="AD216" t="s">
+      <c r="AB216" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="AD216" s="5" t="s">
         <v>698</v>
       </c>
-      <c r="AH216" t="s">
+      <c r="AH216" s="5" t="s">
         <v>721</v>
       </c>
-      <c r="AJ216" t="s">
+      <c r="AJ216" s="5" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="217" spans="1:36" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A217" t="s">
+    <row r="217" spans="1:36" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A217" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B217" t="s">
         <v>60</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C217" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="F217" t="s">
+      <c r="E217"/>
+      <c r="F217" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="G217" t="s">
+      <c r="G217" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="H217" t="s">
+      <c r="H217" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="J217" t="s">
+      <c r="I217"/>
+      <c r="J217" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="L217" t="s">
+      <c r="K217" s="9" t="s">
+        <v>736</v>
+      </c>
+      <c r="L217" s="8" t="s">
         <v>527</v>
       </c>
-      <c r="M217" t="s">
+      <c r="M217" s="8" t="s">
         <v>583</v>
       </c>
-      <c r="N217" t="s">
+      <c r="N217" s="8" t="s">
         <v>623</v>
       </c>
-      <c r="AB217" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="AD217" t="s">
+      <c r="AB217" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="AD217" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="AH217" t="s">
+      <c r="AH217" s="8" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="218" spans="1:36" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A218" t="s">
+    <row r="218" spans="1:36" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A218" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B218" t="s">
         <v>60</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C218" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D218" t="s">
+      <c r="D218" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="F218" t="s">
+      <c r="E218"/>
+      <c r="F218" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="G218" t="s">
+      <c r="G218" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="H218" t="s">
+      <c r="H218" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="J218" t="s">
+      <c r="I218"/>
+      <c r="J218" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="L218" t="s">
+      <c r="K218" s="9" t="s">
+        <v>736</v>
+      </c>
+      <c r="L218" s="8" t="s">
         <v>528</v>
       </c>
-      <c r="M218" t="s">
+      <c r="M218" s="8" t="s">
         <v>583</v>
       </c>
-      <c r="N218" t="s">
+      <c r="N218" s="8" t="s">
         <v>623</v>
       </c>
-      <c r="AB218" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="AD218" t="s">
+      <c r="AB218" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="AD218" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="AH218" t="s">
+      <c r="AH218" s="8" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="219" spans="1:36" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A219" t="s">
+    <row r="219" spans="1:36" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A219" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B219" t="s">
         <v>60</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C219" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D219" t="s">
+      <c r="D219" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="F219" t="s">
+      <c r="E219"/>
+      <c r="F219" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="G219" t="s">
+      <c r="G219" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="H219" t="s">
+      <c r="H219" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="J219" t="s">
+      <c r="I219"/>
+      <c r="J219" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="L219" t="s">
+      <c r="K219" s="9" t="s">
+        <v>736</v>
+      </c>
+      <c r="L219" s="8" t="s">
         <v>529</v>
       </c>
-      <c r="M219" t="s">
+      <c r="M219" s="8" t="s">
         <v>583</v>
       </c>
-      <c r="N219" t="s">
+      <c r="N219" s="8" t="s">
         <v>623</v>
       </c>
-      <c r="AB219" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="AD219" t="s">
+      <c r="AB219" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="AD219" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="AH219" t="s">
+      <c r="AH219" s="8" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="220" spans="1:36" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A220" t="s">
+    <row r="220" spans="1:36" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A220" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B220" t="s">
         <v>60</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C220" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D220" t="s">
+      <c r="D220" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="F220" t="s">
+      <c r="E220"/>
+      <c r="F220" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="G220" t="s">
+      <c r="G220" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="H220" t="s">
+      <c r="H220" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="J220" t="s">
+      <c r="I220"/>
+      <c r="J220" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="L220" t="s">
+      <c r="K220" s="9" t="s">
+        <v>737</v>
+      </c>
+      <c r="L220" s="8" t="s">
         <v>530</v>
       </c>
-      <c r="M220" t="s">
+      <c r="M220" s="8" t="s">
         <v>584</v>
       </c>
-      <c r="N220" t="s">
+      <c r="N220" s="8" t="s">
         <v>624</v>
       </c>
-      <c r="AB220" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="AD220" t="s">
+      <c r="AB220" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="AD220" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="AH220" t="s">
+      <c r="AH220" s="8" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="221" spans="1:36" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A221" t="s">
+    <row r="221" spans="1:36" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A221" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B221" t="s">
         <v>60</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C221" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D221" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="F221" t="s">
+      <c r="E221"/>
+      <c r="F221" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="G221" t="s">
+      <c r="G221" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="H221" t="s">
+      <c r="H221" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="J221" t="s">
+      <c r="I221"/>
+      <c r="J221" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="L221" t="s">
+      <c r="K221" s="9" t="s">
+        <v>738</v>
+      </c>
+      <c r="L221" s="8" t="s">
         <v>531</v>
       </c>
-      <c r="M221" t="s">
+      <c r="M221" s="8" t="s">
         <v>582</v>
       </c>
-      <c r="N221" t="s">
+      <c r="N221" s="8" t="s">
         <v>622</v>
       </c>
-      <c r="AB221" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="AD221" t="s">
+      <c r="AB221" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="AD221" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="AH221" t="s">
+      <c r="AH221" s="8" t="s">
         <v>722</v>
       </c>
     </row>
@@ -12604,6 +12761,9 @@
       <c r="J222" t="s">
         <v>430</v>
       </c>
+      <c r="K222" s="4" t="s">
+        <v>800</v>
+      </c>
       <c r="L222" t="s">
         <v>532</v>
       </c>
@@ -12642,6 +12802,9 @@
       <c r="J223" t="s">
         <v>431</v>
       </c>
+      <c r="K223" s="4" t="s">
+        <v>800</v>
+      </c>
       <c r="L223" t="s">
         <v>532</v>
       </c>
@@ -12680,6 +12843,9 @@
       <c r="J224" t="s">
         <v>432</v>
       </c>
+      <c r="K224" s="4" t="s">
+        <v>801</v>
+      </c>
       <c r="L224" t="s">
         <v>533</v>
       </c>
@@ -12718,6 +12884,9 @@
       <c r="J225" t="s">
         <v>433</v>
       </c>
+      <c r="K225" s="4" t="s">
+        <v>802</v>
+      </c>
       <c r="L225" t="s">
         <v>534</v>
       </c>
@@ -12756,6 +12925,9 @@
       <c r="J226" t="s">
         <v>434</v>
       </c>
+      <c r="K226" s="4" t="s">
+        <v>803</v>
+      </c>
       <c r="L226" t="s">
         <v>535</v>
       </c>
@@ -12794,6 +12966,9 @@
       <c r="J227" t="s">
         <v>435</v>
       </c>
+      <c r="K227" s="4" t="s">
+        <v>804</v>
+      </c>
       <c r="L227" t="s">
         <v>536</v>
       </c>
@@ -12807,223 +12982,253 @@
         <v>714</v>
       </c>
     </row>
-    <row r="228" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A228" t="s">
+    <row r="228" spans="1:34" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A228" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B228" t="s">
         <v>61</v>
       </c>
-      <c r="C228" t="s">
+      <c r="C228" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="F228" t="s">
+      <c r="E228"/>
+      <c r="F228" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="G228" t="s">
+      <c r="G228" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="H228" t="s">
+      <c r="H228" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="J228" t="s">
+      <c r="I228"/>
+      <c r="J228" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="L228" t="s">
+      <c r="K228" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="L228" s="8" t="s">
         <v>537</v>
       </c>
-      <c r="AB228" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="AD228" t="s">
+      <c r="AB228" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="AD228" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="AH228" t="s">
+      <c r="AH228" s="8" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="229" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A229" t="s">
+    <row r="229" spans="1:34" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A229" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B229" t="s">
         <v>61</v>
       </c>
-      <c r="C229" t="s">
+      <c r="C229" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D229" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="F229" t="s">
+      <c r="E229"/>
+      <c r="F229" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="G229" t="s">
+      <c r="G229" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="H229" t="s">
+      <c r="H229" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="J229" t="s">
+      <c r="I229"/>
+      <c r="J229" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="L229" t="s">
+      <c r="K229" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="L229" s="8" t="s">
         <v>537</v>
       </c>
-      <c r="AB229" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="AD229" t="s">
+      <c r="AB229" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="AD229" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="AH229" t="s">
+      <c r="AH229" s="8" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="230" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A230" t="s">
+    <row r="230" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A230" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B230" t="s">
         <v>62</v>
       </c>
-      <c r="C230" t="s">
+      <c r="C230" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D230" t="s">
+      <c r="D230" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F230" t="s">
+      <c r="E230"/>
+      <c r="F230" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="G230" t="s">
+      <c r="G230" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="H230" t="s">
+      <c r="H230" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="J230" t="s">
+      <c r="I230"/>
+      <c r="J230" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="L230" t="s">
+      <c r="K230" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="L230" s="8" t="s">
         <v>538</v>
       </c>
-      <c r="AB230" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="AH230" t="s">
+      <c r="AB230" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="AH230" s="8" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="231" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A231" t="s">
+    <row r="231" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A231" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B231" t="s">
         <v>62</v>
       </c>
-      <c r="C231" t="s">
+      <c r="C231" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D231" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F231" t="s">
+      <c r="E231"/>
+      <c r="F231" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="G231" t="s">
+      <c r="G231" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="H231" t="s">
+      <c r="H231" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="J231" t="s">
+      <c r="I231"/>
+      <c r="J231" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="L231" t="s">
+      <c r="K231" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="L231" s="8" t="s">
         <v>538</v>
       </c>
-      <c r="AB231" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="AH231" t="s">
+      <c r="AB231" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="AH231" s="8" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="232" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A232" t="s">
+    <row r="232" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A232" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B232" t="s">
         <v>62</v>
       </c>
-      <c r="C232" t="s">
+      <c r="C232" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D232" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F232" t="s">
+      <c r="E232"/>
+      <c r="F232" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="G232" t="s">
+      <c r="G232" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="H232" t="s">
+      <c r="H232" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="J232" t="s">
+      <c r="I232"/>
+      <c r="J232" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="L232" t="s">
+      <c r="K232" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="L232" s="8" t="s">
         <v>538</v>
       </c>
-      <c r="AB232" s="3" t="s">
+      <c r="AB232" s="8" t="s">
         <v>693</v>
       </c>
-      <c r="AH232" t="s">
+      <c r="AH232" s="8" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="233" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A233" t="s">
+    <row r="233" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A233" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B233" t="s">
         <v>62</v>
       </c>
-      <c r="C233" t="s">
+      <c r="C233" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D233" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F233" t="s">
+      <c r="E233"/>
+      <c r="F233" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="G233" t="s">
+      <c r="G233" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="H233" t="s">
+      <c r="H233" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="J233" t="s">
+      <c r="I233"/>
+      <c r="J233" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="L233" t="s">
+      <c r="K233" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="L233" s="8" t="s">
         <v>538</v>
       </c>
-      <c r="AB233" s="3" t="s">
+      <c r="AB233" s="8" t="s">
         <v>694</v>
       </c>
-      <c r="AH233" t="s">
+      <c r="AH233" s="8" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="234" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>49</v>
       </c>
@@ -13058,7 +13263,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="235" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>49</v>
       </c>
@@ -13093,7 +13298,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="236" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>49</v>
       </c>
@@ -13128,7 +13333,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="237" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>49</v>
       </c>
@@ -13163,7 +13368,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="238" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>49</v>
       </c>
@@ -13198,7 +13403,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="239" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>49</v>
       </c>
@@ -13233,7 +13438,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="240" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>49</v>
       </c>
@@ -13268,7 +13473,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="241" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>49</v>
       </c>
@@ -13303,7 +13508,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="242" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>49</v>
       </c>
@@ -13338,7 +13543,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="243" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>49</v>
       </c>
@@ -13373,7 +13578,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="244" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>49</v>
       </c>
@@ -13408,7 +13613,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="245" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>49</v>
       </c>
@@ -13443,7 +13648,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="246" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>49</v>
       </c>
@@ -13478,7 +13683,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="247" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>49</v>
       </c>
@@ -13522,7 +13727,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="248" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>49</v>
       </c>
@@ -13566,7 +13771,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="249" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>49</v>
       </c>
@@ -13610,7 +13815,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="250" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>49</v>
       </c>
@@ -13654,7 +13859,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="251" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>49</v>
       </c>
@@ -13698,7 +13903,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="252" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>49</v>
       </c>
@@ -13742,7 +13947,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="253" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>49</v>
       </c>
@@ -13786,7 +13991,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="254" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>49</v>
       </c>
@@ -13830,7 +14035,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="255" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>49</v>
       </c>
@@ -13874,7 +14079,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="256" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>49</v>
       </c>
@@ -13918,7 +14123,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="257" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>49</v>
       </c>
@@ -13962,7 +14167,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="258" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>49</v>
       </c>
@@ -14006,7 +14211,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="259" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>49</v>
       </c>
@@ -14050,7 +14255,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="260" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>49</v>
       </c>
@@ -14094,7 +14299,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="261" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>49</v>
       </c>
@@ -14138,7 +14343,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="262" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>49</v>
       </c>
@@ -14182,7 +14387,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="263" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>49</v>
       </c>
@@ -14226,7 +14431,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="264" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>49</v>
       </c>
@@ -14270,7 +14475,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="265" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>49</v>
       </c>
@@ -14314,7 +14519,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="266" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>49</v>
       </c>
@@ -14355,7 +14560,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="267" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>49</v>
       </c>
@@ -14396,7 +14601,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="268" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>49</v>
       </c>
@@ -14437,7 +14642,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="269" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>49</v>
       </c>
@@ -14481,7 +14686,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="270" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>49</v>
       </c>
@@ -14522,7 +14727,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="271" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>49</v>
       </c>
@@ -14563,7 +14768,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="272" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>49</v>
       </c>
@@ -14604,7 +14809,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="273" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>49</v>
       </c>
@@ -14645,7 +14850,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="274" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>49</v>
       </c>
@@ -14686,7 +14891,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="275" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>49</v>
       </c>
@@ -14727,7 +14932,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="276" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>49</v>
       </c>
@@ -14768,7 +14973,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="277" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>49</v>
       </c>
@@ -14809,7 +15014,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="278" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>49</v>
       </c>
@@ -14850,7 +15055,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="279" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>49</v>
       </c>
@@ -14891,7 +15096,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="280" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>49</v>
       </c>
@@ -14932,7 +15137,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="281" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>49</v>
       </c>
@@ -14973,7 +15178,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="282" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>49</v>
       </c>
@@ -15011,7 +15216,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="283" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>49</v>
       </c>
@@ -15049,7 +15254,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="284" spans="1:34" hidden="1" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>49</v>
       </c>
@@ -15606,7 +15811,7 @@
   <autoFilter ref="A1:AJ296">
     <filterColumn colId="0">
       <filters>
-        <filter val="8"/>
+        <filter val="16"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>